<commit_message>
Updated excel file and xml as per the test name
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\ProspectaLatest\test_automation_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F3473D8-8DE5-4A3A-8A44-2C3509B69238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DB34BD-880E-4CDF-8607-901C579F69E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Workflow_1_TestCases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -531,7 +531,7 @@
   <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Complete workflow testcase 1 with adding all values
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DB34BD-880E-4CDF-8607-901C579F69E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9C43D7-13AA-4893-8ED5-177BC612B2A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Material_type</t>
   </si>
@@ -174,6 +163,12 @@
   </si>
   <si>
     <t>Sales org. 001</t>
+  </si>
+  <si>
+    <t>Ball Bearings</t>
+  </si>
+  <si>
+    <t>Make - To - Order</t>
   </si>
 </sst>
 </file>
@@ -209,10 +204,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +529,7 @@
   <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,8 +656,8 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2">
-        <v>31171504</v>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -667,8 +665,8 @@
       <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Upadted code for automation number field
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9C43D7-13AA-4893-8ED5-177BC612B2A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1791D07E-DB16-4BFB-B43B-8A385C76710F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88246EB4-6BD4-465E-A8ED-E7232FE65B5F}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added new code for expected data in workflow 1
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1791D07E-DB16-4BFB-B43B-8A385C76710F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D52E7-2467-42A3-BB7A-12EFF394D75C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Material_type</t>
   </si>
@@ -169,15 +169,40 @@
   </si>
   <si>
     <t>Make - To - Order</t>
+  </si>
+  <si>
+    <t>BRG,BALL, CR-93101,100MM</t>
+  </si>
+  <si>
+    <t>BRG,BALL,TYPE:ANGULAR DEEP GROOVE,INNER DIAMER:100MM, OUTER DIAMETER:200MM, CAGED MATERIAL:STEEL, CR-93101</t>
+  </si>
+  <si>
+    <t>CREMICA</t>
+  </si>
+  <si>
+    <t>BAG</t>
+  </si>
+  <si>
+    <t>CR2931</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -201,10 +226,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -212,9 +238,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -526,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88246EB4-6BD4-465E-A8ED-E7232FE65B5F}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +566,7 @@
     <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="121.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -551,19 +579,20 @@
     <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.109375" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,40 +645,43 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -701,134 +733,189 @@
       <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" t="s">
         <v>36</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>37</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>38</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>39</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>40</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>41</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>44</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>45</v>
       </c>
       <c r="AB2" t="s">
         <v>45</v>
       </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="3">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3">
+        <v>40</v>
+      </c>
+      <c r="O3" s="3">
+        <v>70</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>9</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>10</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>11</v>
       </c>
-      <c r="M3">
+      <c r="M4">
         <v>12</v>
       </c>
-      <c r="N3">
+      <c r="N4">
         <v>13</v>
       </c>
-      <c r="O3">
+      <c r="O4">
         <v>14</v>
       </c>
-      <c r="P3">
+      <c r="P4">
         <v>15</v>
       </c>
-      <c r="Q3">
+      <c r="Q4">
         <v>16</v>
       </c>
-      <c r="R3">
+      <c r="R4">
         <v>17</v>
       </c>
-      <c r="S3">
+      <c r="S4">
         <v>18</v>
       </c>
-      <c r="T3">
+      <c r="T4">
         <v>19</v>
       </c>
-      <c r="U3">
+      <c r="U4">
         <v>20</v>
       </c>
-      <c r="V3">
+      <c r="V4">
         <v>21</v>
       </c>
-      <c r="W3">
+      <c r="W4">
         <v>22</v>
       </c>
-      <c r="X3">
+      <c r="X4">
         <v>23</v>
       </c>
-      <c r="Y3">
+      <c r="Y4">
         <v>24</v>
       </c>
-      <c r="Z3">
+      <c r="Z4">
         <v>25</v>
       </c>
-      <c r="AA3">
+      <c r="AA4">
         <v>26</v>
       </c>
-      <c r="AB3">
+      <c r="AB4">
         <v>27</v>
       </c>
+      <c r="AC4">
+        <v>28</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="AA14" s="1"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Q15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="AB15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated wait for showing error after submit
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D52E7-2467-42A3-BB7A-12EFF394D75C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659DA98B-C00E-49D8-8211-4DFE34ECF4CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added scroll for visible element
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659DA98B-C00E-49D8-8211-4DFE34ECF4CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA85DE2-1C5E-4CBF-90C4-FDB64D854A25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88246EB4-6BD4-465E-A8ED-E7232FE65B5F}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added test data for workflow 11
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProspectaAutomation\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DB34BD-880E-4CDF-8607-901C579F69E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow_1_TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="Sequential QA (decision + paral" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Material_type</t>
   </si>
@@ -174,12 +174,18 @@
   </si>
   <si>
     <t>Sales org. 001</t>
+  </si>
+  <si>
+    <t>Aut change</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -527,45 +533,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88246EB4-6BD4-465E-A8ED-E7232FE65B5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -737,7 +743,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -823,7 +829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -835,4 +841,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updted excel format from numeric to text
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest_18_08\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89435CAD-B8AB-4682-9644-0E1B52B8034F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow_1_TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Material_type</t>
   </si>
@@ -193,12 +194,42 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +284,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,46 +595,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="121.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="121.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.08984375" customWidth="1"/>
-    <col min="19" max="19" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.109375" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -720,23 +751,23 @@
       <c r="I2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="5">
-        <v>77</v>
-      </c>
-      <c r="K2" s="5">
-        <v>170</v>
-      </c>
-      <c r="L2" s="5">
-        <v>17</v>
-      </c>
-      <c r="M2" s="5">
-        <v>50</v>
+      <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="5">
-        <v>20</v>
+      <c r="O2" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>35</v>
@@ -779,7 +810,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -797,21 +828,21 @@
       <c r="I3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="6">
-        <v>27</v>
-      </c>
-      <c r="K3" s="6">
-        <v>11</v>
-      </c>
-      <c r="L3" s="6">
-        <v>10</v>
-      </c>
-      <c r="M3" s="6">
-        <v>40</v>
+      <c r="J3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="6">
-        <v>70</v>
+      <c r="O3" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>50</v>
@@ -833,7 +864,7 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -922,7 +953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="Q15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -937,21 +968,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Made Changes in Test Data File
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest\test_automation_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProspectaAutomation\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA85DE2-1C5E-4CBF-90C4-FDB64D854A25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D4C33F-54F3-4A61-B956-9CBAB4B618FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow_1_TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="WorkFlow_8_FunctionalLocation" sheetId="2" r:id="rId2"/>
+    <sheet name="WorkFlow_8_AddressMaintaince" sheetId="3" r:id="rId3"/>
+    <sheet name="WorkFlow_8_EquipmentMaster" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="126">
   <si>
     <t>Material_type</t>
   </si>
@@ -187,13 +189,229 @@
   </si>
   <si>
     <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Functional Location Label</t>
+  </si>
+  <si>
+    <t>Edit Mask</t>
+  </si>
+  <si>
+    <t>Labelling System</t>
+  </si>
+  <si>
+    <t>Structure Indicator</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>User status</t>
+  </si>
+  <si>
+    <t>Size / Dimensions</t>
+  </si>
+  <si>
+    <t>Start-Up Date</t>
+  </si>
+  <si>
+    <t>Manufacture Country</t>
+  </si>
+  <si>
+    <t>Model Number</t>
+  </si>
+  <si>
+    <t>Construction Year</t>
+  </si>
+  <si>
+    <t>Manufacturer Serial Number</t>
+  </si>
+  <si>
+    <t>Company Code</t>
+  </si>
+  <si>
+    <t>Business Area</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>Planning Plant</t>
+  </si>
+  <si>
+    <t>Planner Group</t>
+  </si>
+  <si>
+    <t>Maintenance Plant</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Plant Section</t>
+  </si>
+  <si>
+    <t>ABC Indicator</t>
+  </si>
+  <si>
+    <t>Sort Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Record </t>
+  </si>
+  <si>
+    <t>Equipment Installation Allowed</t>
+  </si>
+  <si>
+    <t>Single Equipment Installation</t>
+  </si>
+  <si>
+    <t>MDO5-WS3</t>
+  </si>
+  <si>
+    <t>XXXX-XXX-AA-NN</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Input 40 Char text</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>VIRT</t>
+  </si>
+  <si>
+    <t>12X23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present date </t>
+  </si>
+  <si>
+    <t>ABC PVT LTD</t>
+  </si>
+  <si>
+    <t>AU (Australia)</t>
+  </si>
+  <si>
+    <t>MN12345</t>
+  </si>
+  <si>
+    <t>MPN12345</t>
+  </si>
+  <si>
+    <t>MSN12345</t>
+  </si>
+  <si>
+    <t>BLD</t>
+  </si>
+  <si>
+    <t>MDO SORT TEX</t>
+  </si>
+  <si>
+    <t>Click on "+" icon</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Name</t>
+  </si>
+  <si>
+    <t>Name 2</t>
+  </si>
+  <si>
+    <t>House No</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Street 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country Key</t>
+  </si>
+  <si>
+    <t>City Postal Code</t>
+  </si>
+  <si>
+    <t>Telephone Number</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Fax Number</t>
+  </si>
+  <si>
+    <t>Prospecta</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>UN 206</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irish Tech Park</t>
+  </si>
+  <si>
+    <t>Sector 48</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>xyz@propsecta.com</t>
+  </si>
+  <si>
+    <t>Equipment Category</t>
+  </si>
+  <si>
+    <t>Valid From</t>
+  </si>
+  <si>
+    <t>Valid To</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manufacture Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manufacturer Serial Number: MSN12345</t>
+  </si>
+  <si>
+    <t>16.08.2023</t>
+  </si>
+  <si>
+    <t>31.12.2099</t>
+  </si>
+  <si>
+    <t>12X90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +422,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,11 +459,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,10 +473,31 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -553,46 +808,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88246EB4-6BD4-465E-A8ED-E7232FE65B5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="121.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="121.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.109375" customWidth="1"/>
-    <col min="19" max="19" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.08984375" customWidth="1"/>
+    <col min="19" max="19" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -768,7 +1023,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -819,7 +1074,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -908,7 +1163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="Q15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -920,4 +1175,472 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" s="4"/>
+    </row>
+    <row r="2" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2023</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" s="4">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4">
+        <v>1</v>
+      </c>
+      <c r="W2" s="4">
+        <v>10</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC2" s="4"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="7">
+        <v>122018</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1234567890</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="7">
+        <v>678120</v>
+      </c>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="mailto:xyz@propsecta.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="7">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="7">
+        <v>2023</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created new test for workflow 3
</commit_message>
<xml_diff>
--- a/Test_data1.xlsx
+++ b/Test_data1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\prospecta\prospecta_latest_18_08\test_automation_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89435CAD-B8AB-4682-9644-0E1B52B8034F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98432A-D748-4D0E-BFBB-1B53E45F06B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow_1_TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="Sequential QA (decision + paral" sheetId="2" r:id="rId2"/>
+    <sheet name="Workflow_3_TestCases" sheetId="3" r:id="rId2"/>
+    <sheet name="Sequential QA (decision + paral" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>Material_type</t>
   </si>
@@ -224,6 +225,84 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>Volume Unit</t>
+  </si>
+  <si>
+    <t>Unit of Weight</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>MRP Type</t>
+  </si>
+  <si>
+    <t>Availability Check</t>
+  </si>
+  <si>
+    <t>Profit Centre</t>
+  </si>
+  <si>
+    <t>1st Rem./Exped.</t>
+  </si>
+  <si>
+    <t>2nd Rem./Exped.</t>
+  </si>
+  <si>
+    <t>3rd Rem./Exped.</t>
+  </si>
+  <si>
+    <t>Forecast Model</t>
+  </si>
+  <si>
+    <t>Storage location</t>
+  </si>
+  <si>
+    <t>Valuation Type</t>
+  </si>
+  <si>
+    <t>EA -- Each</t>
+  </si>
+  <si>
+    <t>L -- Liter</t>
+  </si>
+  <si>
+    <t>00101 -- Finished Products</t>
+  </si>
+  <si>
+    <t>KG -- Kilogram</t>
+  </si>
+  <si>
+    <t>0001 -- PLANT 0001</t>
+  </si>
+  <si>
+    <t>ND -- No planning</t>
+  </si>
+  <si>
+    <t>01 -- Daily requirements</t>
+  </si>
+  <si>
+    <t>PC101 -- Profit Centre PC101</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0001 -- M1</t>
+  </si>
+  <si>
+    <t>0001--M1</t>
+  </si>
+  <si>
+    <t>N.A -- N.A</t>
   </si>
 </sst>
 </file>
@@ -598,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
@@ -968,6 +1047,179 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159BF53E-B7E6-4B82-A26C-C5802040F8AA}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10</v>
+      </c>
+      <c r="L3" s="5">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>